<commit_message>
Add SQL schema and update database schema
</commit_message>
<xml_diff>
--- a/Database/Helperland_database.xlsx
+++ b/Database/Helperland_database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\psd-to-html\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C421EED4-70C5-4E0D-921A-AB4863CB253B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F70D32C-5A05-4F61-8D2C-3CEF1688FE2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="881" activeTab="11" xr2:uid="{0FF1C49D-5F74-432D-BAEA-4097385627F9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="881" xr2:uid="{0FF1C49D-5F74-432D-BAEA-4097385627F9}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="84">
   <si>
     <t>UserType</t>
   </si>
@@ -279,9 +279,6 @@
     <t>Servicer</t>
   </si>
   <si>
-    <t>Primary key, Foreign key(Users)</t>
-  </si>
-  <si>
     <t>With_pet</t>
   </si>
   <si>
@@ -292,6 +289,12 @@
   </si>
   <si>
     <t>Is_block</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Foreign key(Users)</t>
+  </si>
+  <si>
+    <t>Id</t>
   </si>
 </sst>
 </file>
@@ -365,16 +368,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -693,7 +696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E827779C-D9DC-4A38-B960-9FC4D8ED086B}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -704,192 +707,196 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11" t="s">
+      <c r="D3" s="9"/>
+      <c r="E3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9" t="s">
+      <c r="B5" s="10"/>
+      <c r="C5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9" t="s">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
     </row>
     <row r="7" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
     </row>
     <row r="12" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9" t="s">
+      <c r="B12" s="10"/>
+      <c r="C12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
     </row>
     <row r="14" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="A3:B4"/>
-    <mergeCell ref="C3:D4"/>
-    <mergeCell ref="E3:G4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="E6:G6"/>
@@ -906,17 +913,13 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="A3:B4"/>
+    <mergeCell ref="C3:D4"/>
+    <mergeCell ref="E3:G4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -928,7 +931,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,11 +942,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -991,7 +994,7 @@
     </row>
     <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>27</v>
@@ -1000,7 +1003,7 @@
     </row>
     <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>27</v>
@@ -1020,7 +1023,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,11 +1034,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -1093,8 +1096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1610F47E-9B64-4087-8F92-F12139B6CDEB}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,11 +1108,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -1199,78 +1202,78 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11" t="s">
+      <c r="D4" s="9"/>
+      <c r="E4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="11"/>
+      <c r="F4" s="9"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9" t="s">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="9"/>
+      <c r="F6" s="10"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1292,10 +1295,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C406A781-451B-4C94-920B-A8025D062BA1}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1304,145 +1307,163 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11" t="s">
+      <c r="D3" s="9"/>
+      <c r="E3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9" t="s">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-    </row>
-    <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9" t="s">
+      <c r="B8" s="10"/>
+      <c r="C8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+    </row>
+    <row r="9" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+    </row>
+    <row r="10" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-    </row>
-    <row r="7" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="9"/>
-    </row>
-    <row r="10" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="9"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="23">
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="A3:B4"/>
+    <mergeCell ref="C3:D4"/>
+    <mergeCell ref="E3:G4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:G7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E8:G8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:G9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="A3:B4"/>
-    <mergeCell ref="C3:D4"/>
-    <mergeCell ref="E3:G4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1454,7 +1475,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1465,31 +1486,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="3"/>
@@ -1498,9 +1519,9 @@
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
       <c r="D4" s="3"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -1599,11 +1620,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -1705,11 +1726,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -1764,7 +1785,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1775,11 +1796,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -1799,7 +1820,9 @@
       <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -1823,7 +1846,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1834,11 +1857,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -1912,7 +1935,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1923,11 +1946,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">

</xml_diff>